<commit_message>
Update data, KMLs and country Excel files
</commit_message>
<xml_diff>
--- a/assets/data/MSME Country Indicators - Bahrain Summary.xlsx
+++ b/assets/data/MSME Country Indicators - Bahrain Summary.xlsx
@@ -31,16 +31,16 @@
     <t>MSMEs</t>
   </si>
   <si>
+    <t>Enterprises density (per 1000 people)</t>
+  </si>
+  <si>
+    <t>38.7</t>
+  </si>
+  <si>
     <t>Enterprises (absolute #)</t>
   </si>
   <si>
     <t>40000</t>
-  </si>
-  <si>
-    <t>Enterprises density (per 1000 people)</t>
-  </si>
-  <si>
-    <t>38.7</t>
   </si>
   <si>
     <t>Enterprises (% of total)</t>

</xml_diff>